<commit_message>
Ref Genome Assembly & Instrument model test cases
</commit_message>
<xml_diff>
--- a/InputFiles/TC04_CDS_Filter_InstrumentModel-Illumina HiSeq.xlsx
+++ b/InputFiles/TC04_CDS_Filter_InstrumentModel-Illumina HiSeq.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kallakuriv2\Automation 0707\Commons_Automation\InputFiles\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F745C708-B1CA-49E2-87B5-C6CAA66A7F5B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68A2350-AB6A-471A-A261-833C2A9BB926}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{8362173B-D28C-47E7-8626-98E16101E601}"/>
   </bookViews>
@@ -57,26 +57,14 @@
     <t>ParticipantsTab</t>
   </si>
   <si>
-    <t>TC01_CDS_Filter_InstrumentModel-DNBSEQ-G400_Neo4jData.xlsx</t>
-  </si>
-  <si>
-    <t>TC01_CDS_Filter_InstrumentModel-DNBSEQ-G400_WebData.xlsx</t>
-  </si>
-  <si>
-    <t>MATCH (f:file)
-Match (f)&lt;--(g:genomic_info)
-WHERE g.instrument_model in ['DNBSEQ-G400']
-MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
-WITH p,f, s, collect(distinct samp.sample_id) as samp
-RETURN
-count(distinct s) AS Studies,
-count(distinct p) AS Participants,
-count(distinct samp) AS Samples,
-count(distinct f) AS Files</t>
+    <t>TC04_CDS_Filter_InstrumentModel-Illumina HiSeq_Neo4jData.xlsx</t>
+  </si>
+  <si>
+    <t>TC04_CDS_Filter_InstrumentModel-Illumina HiSeq_WebData.xlsx</t>
   </si>
   <si>
     <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.instrument_model in ['DNBSEQ-G400']
+WHERE g.instrument_model in ['Illumina HiSeq']
 MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
 WITH p, s, collect(distinct samp.sample_id) as samp
 RETURN 
@@ -89,7 +77,7 @@
   </si>
   <si>
     <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.instrument_model in ['DNBSEQ-G400']
+WHERE g.instrument_model in ['Illumina HiSeq']
 MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
 WITH p,s,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
 RETURN  
@@ -103,7 +91,7 @@
   </si>
   <si>
     <t>Match (f)&lt;--(g:genomic_info)
-WHERE g.instrument_model in ['DNBSEQ-G400']
+WHERE g.instrument_model in ['Illumina HiSeq']
 MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
 WITH p,s,f,samp,COLLECT(DISTINCT samp.sample_tumor_status) as tumor
 RETURN 
@@ -114,6 +102,18 @@
     coalesce(samp.sample_id, '') as `Sample ID`,
     coalesce(f.file_type, '') as `File Type`
 ORDER By f.file_name LIMIT 100</t>
+  </si>
+  <si>
+    <t>MATCH (f:file)
+Match (f)&lt;--(g:genomic_info)
+WHERE g.instrument_model in ['Illumina HiSeq']
+MATCH (f)--&gt;(samp:sample)--&gt;(p:participant)--&gt;(s:study)
+WITH p,f, s, collect(distinct samp.sample_id) as samp
+RETURN
+count(distinct s) AS Studies,
+count(distinct p) AS Participants,
+count(distinct samp) AS Samples,
+count(distinct f) AS Files</t>
   </si>
 </sst>
 </file>
@@ -494,7 +494,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A2" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="21" x14ac:dyDescent="0.35"/>
@@ -502,7 +502,7 @@
     <col min="1" max="1" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="96.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="74.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="78.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="88.28515625" style="1" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="85.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
@@ -529,10 +529,10 @@
         <v>7</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>8</v>
@@ -546,10 +546,10 @@
         <v>5</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" s="2" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D3" s="1" t="s">
         <v>8</v>
@@ -563,10 +563,10 @@
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>13</v>
-      </c>
-      <c r="C4" s="2" t="s">
-        <v>10</v>
       </c>
       <c r="D4" s="1" t="s">
         <v>8</v>

</xml_diff>